<commit_message>
fixing pop.xml and updating some test data for the ai driven test
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/dashboards_ScreenshotsComparer/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/dashboards_ScreenshotsComparer/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -44,19 +44,22 @@
     <t xml:space="preserve">URL_login_login</t>
   </si>
   <si>
-    <t xml:space="preserve">new/login</t>
+    <t xml:space="preserve">#/login</t>
   </si>
   <si>
     <t xml:space="preserve">URL_content</t>
   </si>
   <si>
-    <t xml:space="preserve">new/catalog</t>
+    <t xml:space="preserve">#/catalog</t>
   </si>
   <si>
     <t xml:space="preserve">User Credentials</t>
   </si>
   <si>
     <t xml:space="preserve">Tenant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">security</t>
   </si>
   <si>
     <t xml:space="preserve">NewUI</t>
@@ -296,7 +299,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -478,7 +481,9 @@
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -505,10 +510,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -537,10 +542,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -569,7 +574,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1626,7 +1631,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1656,7 +1661,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1686,7 +1691,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1716,7 +1721,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1746,7 +1751,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>

</xml_diff>

<commit_message>
Committing the dashboard crawler for execution
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/dashboards_ScreenshotsComparer/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/dashboards_ScreenshotsComparer/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tenant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">security</t>
   </si>
   <si>
     <t xml:space="preserve">NewUI</t>
@@ -299,7 +296,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -481,9 +478,6 @@
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -510,10 +504,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -542,10 +536,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -574,7 +568,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1618,7 +1612,7 @@
   <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1631,7 +1625,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1661,7 +1655,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1691,7 +1685,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1721,7 +1715,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1751,7 +1745,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>

</xml_diff>

<commit_message>
fixes and performance boosters for the dashboardCrawler
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/dashboards_ScreenshotsComparer/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/dashboards_ScreenshotsComparer/TestData.xlsx
@@ -44,13 +44,13 @@
     <t xml:space="preserve">URL_login_login</t>
   </si>
   <si>
-    <t xml:space="preserve">login</t>
+    <t xml:space="preserve">#/login</t>
   </si>
   <si>
     <t xml:space="preserve">URL_content</t>
   </si>
   <si>
-    <t xml:space="preserve">catalog</t>
+    <t xml:space="preserve">#/catalog</t>
   </si>
   <si>
     <t xml:space="preserve">User Credentials</t>
@@ -296,7 +296,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1612,7 +1612,7 @@
   <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
modifying to run with keysight
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/dashboards_ScreenshotsComparer/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/dashboards_ScreenshotsComparer/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -59,16 +59,19 @@
     <t xml:space="preserve">Tenant</t>
   </si>
   <si>
-    <t xml:space="preserve">ebs</t>
+    <t xml:space="preserve">siebel</t>
   </si>
   <si>
     <t xml:space="preserve">Username</t>
   </si>
   <si>
-    <t xml:space="preserve">admin</t>
+    <t xml:space="preserve">super</t>
   </si>
   <si>
     <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin</t>
   </si>
   <si>
     <t xml:space="preserve">Dashboard Crawler…</t>
@@ -539,7 +542,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -568,7 +571,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1625,7 +1628,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1655,7 +1658,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1685,7 +1688,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1715,7 +1718,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1745,7 +1748,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>

</xml_diff>

<commit_message>
updating test data for ingen2 run
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/dashboards_ScreenshotsComparer/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/dashboards_ScreenshotsComparer/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -59,19 +59,16 @@
     <t xml:space="preserve">Tenant</t>
   </si>
   <si>
-    <t xml:space="preserve">siebel</t>
+    <t xml:space="preserve">ingen2</t>
   </si>
   <si>
     <t xml:space="preserve">Username</t>
   </si>
   <si>
-    <t xml:space="preserve">super</t>
+    <t xml:space="preserve">admin</t>
   </si>
   <si>
     <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin</t>
   </si>
   <si>
     <t xml:space="preserve">Dashboard Crawler…</t>
@@ -542,7 +539,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -571,7 +568,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1628,7 +1625,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1658,7 +1655,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1688,7 +1685,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1718,7 +1715,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1748,7 +1745,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>

</xml_diff>